<commit_message>
criação de novos campos
</commit_message>
<xml_diff>
--- a/src/planilha/planilha_nfse.xlsx
+++ b/src/planilha/planilha_nfse.xlsx
@@ -124,7 +124,7 @@
     <t xml:space="preserve">ir</t>
   </si>
   <si>
-    <t xml:space="preserve">52</t>
+    <t xml:space="preserve">40028922</t>
   </si>
   <si>
     <t xml:space="preserve">U</t>
@@ -136,28 +136,28 @@
     <t xml:space="preserve">NÃO</t>
   </si>
   <si>
+    <t xml:space="preserve">SIM</t>
+  </si>
+  <si>
     <t xml:space="preserve">07.02</t>
   </si>
   <si>
     <t xml:space="preserve">43.456.133/0001-80</t>
   </si>
   <si>
-    <t xml:space="preserve">POLIMIX CONCRETO LTDA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29.067.113/0239-94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERRA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CONCRETO USIN FCK15 B0/1 10+/-2CM LOG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAO</t>
+    <t xml:space="preserve">JOAO ANTONIO PEREIRA GONCALVES EMPR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.675.476/0001-86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BELO HORIZONTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SERVICO DE FUNDACAO - TRADO MECANIZADO S</t>
   </si>
 </sst>
 </file>
@@ -171,7 +171,7 @@
     <numFmt numFmtId="167" formatCode="#,##0.00"/>
     <numFmt numFmtId="168" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -198,11 +198,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -260,44 +255,40 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,8 +543,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9140625" defaultRowHeight="12" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -582,7 +573,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="7.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="12.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -691,10 +682,10 @@
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>45713</v>
+        <v>46077</v>
       </c>
       <c r="B2" s="4" t="n">
-        <v>46029</v>
+        <v>46077</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>34</v>
@@ -709,94 +700,79 @@
         <v>37</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R2" s="6" t="n">
-        <v>3537701</v>
+        <v>3201308</v>
       </c>
       <c r="S2" s="6" t="n">
-        <v>3537701</v>
-      </c>
-      <c r="T2" s="7" t="n">
         <v>3201308</v>
       </c>
-      <c r="U2" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V2" s="8"/>
+      <c r="T2" s="6" t="n">
+        <v>3201308</v>
+      </c>
+      <c r="U2" s="7" t="n">
+        <v>5</v>
+      </c>
+      <c r="V2" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="W2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="X2" s="8" t="n">
-        <v>2064.35</v>
-      </c>
-      <c r="Y2" s="8" t="n">
+        <v>45</v>
+      </c>
+      <c r="X2" s="7" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="Y2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="Z2" s="8" t="n">
+      <c r="Z2" s="7" t="n">
         <v>7.02</v>
       </c>
-      <c r="AA2" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB2" s="8"/>
-      <c r="AC2" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD2" s="8" t="n">
+      <c r="AA2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB2" s="7"/>
+      <c r="AC2" s="8" t="n">
+        <v>4.76</v>
+      </c>
+      <c r="AD2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="AE2" s="8" t="n">
+      <c r="AE2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="AF2" s="8" t="n">
+      <c r="AF2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="AG2" s="8" t="n">
+      <c r="AG2" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="AH2" s="8" t="n">
-        <v>0</v>
+      <c r="AH2" s="7" t="n">
+        <v>369.26</v>
       </c>
     </row>
-    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>